<commit_message>
Change radius of all buttons
</commit_message>
<xml_diff>
--- a/Documents/하늘보리 일일 회의록.xlsx
+++ b/Documents/하늘보리 일일 회의록.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joey3\HB\HaneulBori\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwontaewoo/Documents/M@TAEWOO$/Programming/Git/HaneulBori/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043C6C32-B954-49AB-86B5-8C69319AFBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF4C059-8790-804A-8AE4-CAC8EFB658D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="product backlog" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="76">
   <si>
     <t>예약</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -468,19 +468,27 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Firebase 연동 전 사용자 및 세탁기 정보를  
+class 생성 후 데이터 자체저장 작업</t>
+  </si>
+  <si>
+    <t>1. 예략 버튼 세탁기별 1개에서 
+통합된 버튼 1개로 수정 
+2. Firebase Firestore 활용하여 
+Swift 프로젝트와 연동</t>
+  </si>
+  <si>
     <t>없음</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1018,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1188,63 +1196,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1461,40 +1475,40 @@
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14" thickBot="1">
       <c r="A4" s="3"/>
       <c r="B4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="73" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A5" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="D5" s="74" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="74"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="78"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
+      <c r="A6" s="69"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="75"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1">
       <c r="A7" s="8">
         <v>1</v>
       </c>
@@ -1509,7 +1523,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="A8" s="6">
         <v>2</v>
       </c>
@@ -1524,7 +1538,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1">
       <c r="A9" s="6">
         <v>3</v>
       </c>
@@ -1539,7 +1553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1">
       <c r="A10" s="6">
         <v>4</v>
       </c>
@@ -1554,7 +1568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1">
       <c r="A11" s="6">
         <v>5</v>
       </c>
@@ -1572,7 +1586,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" thickBot="1">
       <c r="A12" s="7">
         <v>6</v>
       </c>
@@ -1591,28 +1605,28 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="65" t="s">
+    <row r="13" spans="1:5" ht="14" thickBot="1"/>
+    <row r="14" spans="1:5">
+      <c r="A14" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="69" t="s">
+      <c r="C14" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="80" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="66"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="72"/>
-    </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="14" thickBot="1">
+      <c r="A15" s="77"/>
+      <c r="B15" s="79"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="81"/>
+    </row>
+    <row r="16" spans="1:5" ht="15">
       <c r="A16" s="8">
         <v>1</v>
       </c>
@@ -1627,7 +1641,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="14">
       <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>17</v>
@@ -1639,7 +1653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="14">
       <c r="A18" s="23"/>
       <c r="B18" s="4" t="s">
         <v>18</v>
@@ -1651,7 +1665,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="14">
       <c r="A19" s="23"/>
       <c r="B19" s="4" t="s">
         <v>21</v>
@@ -1663,46 +1677,46 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="14">
       <c r="A20" s="23"/>
       <c r="B20" s="4"/>
       <c r="C20" s="20"/>
       <c r="D20" s="16"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="14">
       <c r="A21" s="23"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
       <c r="D21" s="16"/>
     </row>
-    <row r="22" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15" thickBot="1">
       <c r="A22" s="24"/>
       <c r="B22" s="13"/>
       <c r="C22" s="14"/>
       <c r="D22" s="18"/>
     </row>
-    <row r="23" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+    <row r="23" spans="1:4" ht="14" thickBot="1"/>
+    <row r="24" spans="1:4">
+      <c r="A24" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="69" t="s">
+      <c r="C24" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="71" t="s">
+      <c r="D24" s="80" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="66"/>
-      <c r="B25" s="68"/>
-      <c r="C25" s="70"/>
-      <c r="D25" s="72"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="14" thickBot="1">
+      <c r="A25" s="77"/>
+      <c r="B25" s="79"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="81"/>
+    </row>
+    <row r="26" spans="1:4" ht="14">
       <c r="A26" s="6">
         <v>2</v>
       </c>
@@ -1717,7 +1731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15">
       <c r="A27" s="25"/>
       <c r="B27" s="5" t="s">
         <v>26</v>
@@ -1729,7 +1743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="14">
       <c r="A28" s="23"/>
       <c r="B28" s="4" t="s">
         <v>23</v>
@@ -1741,7 +1755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="14">
       <c r="A29" s="23"/>
       <c r="B29" s="4" t="s">
         <v>28</v>
@@ -1753,44 +1767,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4">
       <c r="A30" s="23"/>
       <c r="D30" s="16"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="14">
       <c r="A31" s="23"/>
       <c r="B31" s="11"/>
       <c r="C31" s="12"/>
       <c r="D31" s="16"/>
     </row>
-    <row r="32" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="15" thickBot="1">
       <c r="A32" s="24"/>
       <c r="B32" s="13"/>
       <c r="C32" s="14"/>
       <c r="D32" s="18"/>
     </row>
-    <row r="33" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="65" t="s">
+    <row r="33" spans="1:4" ht="14" thickBot="1"/>
+    <row r="34" spans="1:4">
+      <c r="A34" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="67" t="s">
+      <c r="B34" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="69" t="s">
+      <c r="C34" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="71" t="s">
+      <c r="D34" s="80" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="66"/>
-      <c r="B35" s="68"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="72"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="14" thickBot="1">
+      <c r="A35" s="77"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="73"/>
+      <c r="D35" s="81"/>
+    </row>
+    <row r="36" spans="1:4" ht="14">
       <c r="A36" s="6">
         <v>3</v>
       </c>
@@ -1805,7 +1819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="14">
       <c r="A37" s="25"/>
       <c r="B37" s="11" t="s">
         <v>0</v>
@@ -1817,7 +1831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="14">
       <c r="A38" s="23"/>
       <c r="B38" s="4" t="s">
         <v>1</v>
@@ -1829,52 +1843,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="14">
       <c r="A39" s="23"/>
       <c r="B39" s="4"/>
       <c r="C39" s="20"/>
       <c r="D39" s="16"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="23"/>
       <c r="B40" s="21"/>
       <c r="C40" s="21"/>
       <c r="D40" s="16"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="14">
       <c r="A41" s="23"/>
       <c r="B41" s="11"/>
       <c r="C41" s="12"/>
       <c r="D41" s="16"/>
     </row>
-    <row r="42" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15" thickBot="1">
       <c r="A42" s="24"/>
       <c r="B42" s="13"/>
       <c r="C42" s="14"/>
       <c r="D42" s="18"/>
     </row>
-    <row r="43" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="65" t="s">
+    <row r="43" spans="1:4" ht="14" thickBot="1"/>
+    <row r="44" spans="1:4">
+      <c r="A44" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="67" t="s">
+      <c r="B44" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="69" t="s">
+      <c r="C44" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="71" t="s">
+      <c r="D44" s="80" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="66"/>
-      <c r="B45" s="68"/>
-      <c r="C45" s="70"/>
-      <c r="D45" s="72"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="14" thickBot="1">
+      <c r="A45" s="77"/>
+      <c r="B45" s="79"/>
+      <c r="C45" s="73"/>
+      <c r="D45" s="81"/>
+    </row>
+    <row r="46" spans="1:4" ht="14">
       <c r="A46" s="6">
         <v>4</v>
       </c>
@@ -1889,7 +1903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="14">
       <c r="A47" s="25"/>
       <c r="B47" s="11" t="s">
         <v>32</v>
@@ -1901,7 +1915,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="14">
       <c r="A48" s="23"/>
       <c r="B48" s="4" t="s">
         <v>34</v>
@@ -1913,52 +1927,52 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="14">
       <c r="A49" s="23"/>
       <c r="B49" s="4"/>
       <c r="C49" s="20"/>
       <c r="D49" s="16"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="23"/>
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
       <c r="D50" s="16"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="14">
       <c r="A51" s="23"/>
       <c r="B51" s="11"/>
       <c r="C51" s="12"/>
       <c r="D51" s="16"/>
     </row>
-    <row r="52" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15" thickBot="1">
       <c r="A52" s="24"/>
       <c r="B52" s="13"/>
       <c r="C52" s="14"/>
       <c r="D52" s="18"/>
     </row>
-    <row r="53" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="73" t="s">
+    <row r="53" spans="1:4" ht="14" thickBot="1"/>
+    <row r="54" spans="1:4">
+      <c r="A54" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="75" t="s">
+      <c r="B54" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C54" s="69" t="s">
+      <c r="C54" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="77" t="s">
+      <c r="D54" s="74" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="74"/>
-      <c r="B55" s="76"/>
-      <c r="C55" s="70"/>
-      <c r="D55" s="78"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="14" thickBot="1">
+      <c r="A55" s="69"/>
+      <c r="B55" s="71"/>
+      <c r="C55" s="73"/>
+      <c r="D55" s="75"/>
+    </row>
+    <row r="56" spans="1:4" ht="14">
       <c r="A56" s="6">
         <v>5</v>
       </c>
@@ -1973,7 +1987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="14">
       <c r="A57" s="6"/>
       <c r="B57" s="5" t="s">
         <v>36</v>
@@ -1985,58 +1999,58 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="14">
       <c r="A58" s="6"/>
       <c r="B58" s="4"/>
       <c r="C58" s="10"/>
       <c r="D58" s="17"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="14">
       <c r="A59" s="6"/>
       <c r="B59" s="4"/>
       <c r="C59" s="10"/>
       <c r="D59" s="16"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="14">
       <c r="A60" s="6"/>
       <c r="B60" s="4"/>
       <c r="C60" s="20"/>
       <c r="D60" s="16"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="14">
       <c r="A61" s="6"/>
       <c r="B61" s="11"/>
       <c r="C61" s="12"/>
       <c r="D61" s="16"/>
     </row>
-    <row r="62" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15" thickBot="1">
       <c r="A62" s="7"/>
       <c r="B62" s="13"/>
       <c r="C62" s="14"/>
       <c r="D62" s="18"/>
     </row>
-    <row r="63" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="73" t="s">
+    <row r="63" spans="1:4" ht="14" thickBot="1"/>
+    <row r="64" spans="1:4">
+      <c r="A64" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="75" t="s">
+      <c r="B64" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C64" s="69" t="s">
+      <c r="C64" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D64" s="77" t="s">
+      <c r="D64" s="74" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="74"/>
-      <c r="B65" s="76"/>
-      <c r="C65" s="70"/>
-      <c r="D65" s="78"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="14" thickBot="1">
+      <c r="A65" s="69"/>
+      <c r="B65" s="71"/>
+      <c r="C65" s="73"/>
+      <c r="D65" s="75"/>
+    </row>
+    <row r="66" spans="1:4" ht="14">
       <c r="A66" s="31">
         <v>6</v>
       </c>
@@ -2051,7 +2065,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="14">
       <c r="A67" s="27"/>
       <c r="B67" s="28" t="s">
         <v>38</v>
@@ -2063,7 +2077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="14">
       <c r="A68" s="6"/>
       <c r="B68" s="4" t="s">
         <v>39</v>
@@ -2075,25 +2089,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="14">
       <c r="A69" s="6"/>
       <c r="B69" s="4"/>
       <c r="C69" s="10"/>
       <c r="D69" s="16"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="14">
       <c r="A70" s="6"/>
       <c r="B70" s="4"/>
       <c r="C70" s="20"/>
       <c r="D70" s="16"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="14">
       <c r="A71" s="6"/>
       <c r="B71" s="11"/>
       <c r="C71" s="12"/>
       <c r="D71" s="16"/>
     </row>
-    <row r="72" spans="1:4" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" ht="15" thickBot="1">
       <c r="A72" s="7"/>
       <c r="B72" s="13"/>
       <c r="C72" s="14"/>
@@ -2101,6 +2115,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
     <mergeCell ref="A64:A65"/>
     <mergeCell ref="B64:B65"/>
     <mergeCell ref="C64:C65"/>
@@ -2113,22 +2143,6 @@
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="C54:C55"/>
     <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2140,24 +2154,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6478D81-E9A2-AE49-B0C1-A9177BDCDC72}">
   <dimension ref="B3:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" customWidth="1"/>
     <col min="4" max="6" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="14" thickBot="1"/>
+    <row r="4" spans="2:6" ht="14" thickBot="1">
       <c r="B4" s="44" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="50" t="s">
         <v>42</v>
       </c>
@@ -2174,7 +2188,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="80" customHeight="1">
       <c r="B6" s="42" t="s">
         <v>46</v>
       </c>
@@ -2182,68 +2196,68 @@
         <v>61</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="F6" s="67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="80" customHeight="1">
       <c r="B7" s="42" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="80" customHeight="1">
       <c r="B8" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B9" s="43" t="s">
         <v>49</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D9" s="63" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E9" s="63" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F9" s="64" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="14" thickBot="1"/>
+    <row r="13" spans="2:6" ht="14" thickBot="1">
       <c r="B13" s="44" t="s">
         <v>63</v>
       </c>
@@ -2252,7 +2266,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" s="50" t="s">
         <v>42</v>
       </c>
@@ -2269,7 +2283,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="80" customHeight="1">
       <c r="B15" s="42" t="s">
         <v>46</v>
       </c>
@@ -2277,68 +2291,68 @@
         <v>61</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="82" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="F15" s="67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="80" customHeight="1">
       <c r="B16" s="42" t="s">
         <v>47</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="80" customHeight="1">
       <c r="B17" s="42" t="s">
         <v>48</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B18" s="43" t="s">
         <v>49</v>
       </c>
       <c r="C18" s="62" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="E18" s="63" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F18" s="64" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="14" thickBot="1"/>
+    <row r="22" spans="2:6" ht="14" thickBot="1">
       <c r="B22" s="44" t="s">
         <v>50</v>
       </c>
@@ -2347,7 +2361,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="50" t="s">
         <v>42</v>
       </c>
@@ -2364,31 +2378,41 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="80" customHeight="1">
       <c r="B24" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="46"/>
-    </row>
-    <row r="25" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="83" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="84" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="80" customHeight="1">
       <c r="B25" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="79" t="s">
+      <c r="C25" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="D25" s="81" t="s">
+      <c r="D25" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="80" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="46"/>
-    </row>
-    <row r="26" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="80" customHeight="1">
       <c r="B26" s="42" t="s">
         <v>48</v>
       </c>
@@ -2397,7 +2421,7 @@
       <c r="E26" s="36"/>
       <c r="F26" s="46"/>
     </row>
-    <row r="27" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B27" s="43" t="s">
         <v>49</v>
       </c>
@@ -2406,8 +2430,8 @@
       <c r="E27" s="48"/>
       <c r="F27" s="49"/>
     </row>
-    <row r="30" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="14" thickBot="1"/>
+    <row r="31" spans="2:6" ht="14" thickBot="1">
       <c r="B31" s="52" t="s">
         <v>64</v>
       </c>
@@ -2418,7 +2442,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6">
       <c r="B32" s="50" t="s">
         <v>42</v>
       </c>
@@ -2435,7 +2459,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="80" customHeight="1">
       <c r="B33" s="42" t="s">
         <v>46</v>
       </c>
@@ -2444,7 +2468,7 @@
       <c r="E33" s="36"/>
       <c r="F33" s="46"/>
     </row>
-    <row r="34" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="80" customHeight="1">
       <c r="B34" s="42" t="s">
         <v>47</v>
       </c>
@@ -2453,7 +2477,7 @@
       <c r="E34" s="36"/>
       <c r="F34" s="46"/>
     </row>
-    <row r="35" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="80" customHeight="1">
       <c r="B35" s="42" t="s">
         <v>48</v>
       </c>
@@ -2462,7 +2486,7 @@
       <c r="E35" s="36"/>
       <c r="F35" s="46"/>
     </row>
-    <row r="36" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B36" s="43" t="s">
         <v>49</v>
       </c>
@@ -2471,8 +2495,8 @@
       <c r="E36" s="48"/>
       <c r="F36" s="49"/>
     </row>
-    <row r="39" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="14" thickBot="1"/>
+    <row r="40" spans="2:6" ht="14" thickBot="1">
       <c r="B40" s="52" t="s">
         <v>52</v>
       </c>
@@ -2483,7 +2507,7 @@
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6">
       <c r="B41" s="50" t="s">
         <v>42</v>
       </c>
@@ -2500,7 +2524,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" ht="80" customHeight="1">
       <c r="B42" s="42" t="s">
         <v>46</v>
       </c>
@@ -2509,7 +2533,7 @@
       <c r="E42" s="35"/>
       <c r="F42" s="57"/>
     </row>
-    <row r="43" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="80" customHeight="1">
       <c r="B43" s="42" t="s">
         <v>47</v>
       </c>
@@ -2518,7 +2542,7 @@
       <c r="E43" s="35"/>
       <c r="F43" s="57"/>
     </row>
-    <row r="44" spans="2:6" ht="67.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" ht="68" customHeight="1">
       <c r="B44" s="42" t="s">
         <v>48</v>
       </c>
@@ -2527,7 +2551,7 @@
       <c r="E44" s="35"/>
       <c r="F44" s="57"/>
     </row>
-    <row r="45" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B45" s="43" t="s">
         <v>49</v>
       </c>
@@ -2551,22 +2575,22 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="22"/>
+    <col min="1" max="1" width="10.83203125" style="22"/>
     <col min="2" max="2" width="16.6640625" style="22" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" style="22" customWidth="1"/>
     <col min="4" max="6" width="25" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="10.77734375" style="22"/>
+    <col min="7" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="14" thickBot="1"/>
+    <row r="4" spans="2:6" ht="14" thickBot="1">
       <c r="B4" s="44" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="50" t="s">
         <v>42</v>
       </c>
@@ -2583,7 +2607,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="80" customHeight="1">
       <c r="B6" s="42" t="s">
         <v>46</v>
       </c>
@@ -2592,7 +2616,7 @@
       <c r="E6" s="36"/>
       <c r="F6" s="46"/>
     </row>
-    <row r="7" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="80" customHeight="1">
       <c r="B7" s="42" t="s">
         <v>47</v>
       </c>
@@ -2601,7 +2625,7 @@
       <c r="E7" s="36"/>
       <c r="F7" s="46"/>
     </row>
-    <row r="8" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="80" customHeight="1">
       <c r="B8" s="42" t="s">
         <v>48</v>
       </c>
@@ -2610,7 +2634,7 @@
       <c r="E8" s="36"/>
       <c r="F8" s="46"/>
     </row>
-    <row r="9" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B9" s="43" t="s">
         <v>49</v>
       </c>
@@ -2619,13 +2643,13 @@
       <c r="E9" s="48"/>
       <c r="F9" s="49"/>
     </row>
-    <row r="12" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="14" thickBot="1"/>
+    <row r="13" spans="2:6" ht="14" thickBot="1">
       <c r="B13" s="44" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" s="50" t="s">
         <v>42</v>
       </c>
@@ -2642,7 +2666,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="80" customHeight="1">
       <c r="B15" s="42" t="s">
         <v>46</v>
       </c>
@@ -2651,7 +2675,7 @@
       <c r="E15" s="36"/>
       <c r="F15" s="46"/>
     </row>
-    <row r="16" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="80" customHeight="1">
       <c r="B16" s="42" t="s">
         <v>47</v>
       </c>
@@ -2660,7 +2684,7 @@
       <c r="E16" s="36"/>
       <c r="F16" s="46"/>
     </row>
-    <row r="17" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="80" customHeight="1">
       <c r="B17" s="42" t="s">
         <v>48</v>
       </c>
@@ -2669,7 +2693,7 @@
       <c r="E17" s="36"/>
       <c r="F17" s="46"/>
     </row>
-    <row r="18" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B18" s="43" t="s">
         <v>49</v>
       </c>
@@ -2678,13 +2702,13 @@
       <c r="E18" s="48"/>
       <c r="F18" s="49"/>
     </row>
-    <row r="21" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="14" thickBot="1"/>
+    <row r="22" spans="2:6" ht="14" thickBot="1">
       <c r="B22" s="44" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="50" t="s">
         <v>42</v>
       </c>
@@ -2701,7 +2725,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="80" customHeight="1">
       <c r="B24" s="42" t="s">
         <v>46</v>
       </c>
@@ -2710,7 +2734,7 @@
       <c r="E24" s="36"/>
       <c r="F24" s="46"/>
     </row>
-    <row r="25" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="80" customHeight="1">
       <c r="B25" s="42" t="s">
         <v>47</v>
       </c>
@@ -2719,7 +2743,7 @@
       <c r="E25" s="36"/>
       <c r="F25" s="46"/>
     </row>
-    <row r="26" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="80" customHeight="1">
       <c r="B26" s="42" t="s">
         <v>48</v>
       </c>
@@ -2728,7 +2752,7 @@
       <c r="E26" s="36"/>
       <c r="F26" s="46"/>
     </row>
-    <row r="27" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B27" s="43" t="s">
         <v>49</v>
       </c>
@@ -2737,14 +2761,14 @@
       <c r="E27" s="48"/>
       <c r="F27" s="49"/>
     </row>
-    <row r="30" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="14" thickBot="1"/>
+    <row r="31" spans="2:6" ht="14" thickBot="1">
       <c r="B31" s="44" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="54"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6">
       <c r="B32" s="55" t="s">
         <v>42</v>
       </c>
@@ -2761,7 +2785,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="80" customHeight="1">
       <c r="B33" s="42" t="s">
         <v>46</v>
       </c>
@@ -2770,7 +2794,7 @@
       <c r="E33" s="36"/>
       <c r="F33" s="46"/>
     </row>
-    <row r="34" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="80" customHeight="1">
       <c r="B34" s="42" t="s">
         <v>47</v>
       </c>
@@ -2779,7 +2803,7 @@
       <c r="E34" s="36"/>
       <c r="F34" s="46"/>
     </row>
-    <row r="35" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="80" customHeight="1">
       <c r="B35" s="42" t="s">
         <v>48</v>
       </c>
@@ -2788,7 +2812,7 @@
       <c r="E35" s="36"/>
       <c r="F35" s="46"/>
     </row>
-    <row r="36" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B36" s="43" t="s">
         <v>49</v>
       </c>
@@ -2797,14 +2821,14 @@
       <c r="E36" s="48"/>
       <c r="F36" s="49"/>
     </row>
-    <row r="39" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="14" thickBot="1"/>
+    <row r="40" spans="2:6" ht="14" thickBot="1">
       <c r="B40" s="44" t="s">
         <v>59</v>
       </c>
       <c r="C40" s="54"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6">
       <c r="B41" s="55" t="s">
         <v>42</v>
       </c>
@@ -2821,7 +2845,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" ht="80" customHeight="1">
       <c r="B42" s="42" t="s">
         <v>46</v>
       </c>
@@ -2830,7 +2854,7 @@
       <c r="E42" s="36"/>
       <c r="F42" s="46"/>
     </row>
-    <row r="43" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="80" customHeight="1">
       <c r="B43" s="42" t="s">
         <v>47</v>
       </c>
@@ -2839,7 +2863,7 @@
       <c r="E43" s="36"/>
       <c r="F43" s="46"/>
     </row>
-    <row r="44" spans="2:6" ht="67.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" ht="68" customHeight="1">
       <c r="B44" s="42" t="s">
         <v>48</v>
       </c>
@@ -2848,7 +2872,7 @@
       <c r="E44" s="36"/>
       <c r="F44" s="46"/>
     </row>
-    <row r="45" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B45" s="43" t="s">
         <v>49</v>
       </c>
@@ -2871,22 +2895,22 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="22"/>
+    <col min="1" max="1" width="10.83203125" style="22"/>
     <col min="2" max="2" width="16.6640625" style="22" customWidth="1"/>
     <col min="3" max="3" width="41.6640625" style="22" customWidth="1"/>
     <col min="4" max="6" width="25" style="22" customWidth="1"/>
-    <col min="7" max="16384" width="10.77734375" style="22"/>
+    <col min="7" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="14" thickBot="1"/>
+    <row r="4" spans="2:6" ht="14" thickBot="1">
       <c r="B4" s="44" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6">
       <c r="B5" s="50" t="s">
         <v>42</v>
       </c>
@@ -2903,7 +2927,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="80" customHeight="1">
       <c r="B6" s="42" t="s">
         <v>46</v>
       </c>
@@ -2912,7 +2936,7 @@
       <c r="E6" s="36"/>
       <c r="F6" s="46"/>
     </row>
-    <row r="7" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="80" customHeight="1">
       <c r="B7" s="42" t="s">
         <v>47</v>
       </c>
@@ -2921,7 +2945,7 @@
       <c r="E7" s="36"/>
       <c r="F7" s="46"/>
     </row>
-    <row r="8" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="80" customHeight="1">
       <c r="B8" s="42" t="s">
         <v>48</v>
       </c>
@@ -2930,7 +2954,7 @@
       <c r="E8" s="36"/>
       <c r="F8" s="46"/>
     </row>
-    <row r="9" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B9" s="43" t="s">
         <v>49</v>
       </c>
@@ -2939,13 +2963,13 @@
       <c r="E9" s="48"/>
       <c r="F9" s="49"/>
     </row>
-    <row r="12" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="14" thickBot="1"/>
+    <row r="13" spans="2:6" ht="14" thickBot="1">
       <c r="B13" s="44" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6">
       <c r="B14" s="50" t="s">
         <v>42</v>
       </c>
@@ -2962,7 +2986,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="80" customHeight="1">
       <c r="B15" s="42" t="s">
         <v>46</v>
       </c>
@@ -2971,7 +2995,7 @@
       <c r="E15" s="36"/>
       <c r="F15" s="46"/>
     </row>
-    <row r="16" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="80" customHeight="1">
       <c r="B16" s="42" t="s">
         <v>47</v>
       </c>
@@ -2980,7 +3004,7 @@
       <c r="E16" s="36"/>
       <c r="F16" s="46"/>
     </row>
-    <row r="17" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" ht="80" customHeight="1">
       <c r="B17" s="42" t="s">
         <v>48</v>
       </c>
@@ -2989,7 +3013,7 @@
       <c r="E17" s="36"/>
       <c r="F17" s="46"/>
     </row>
-    <row r="18" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B18" s="43" t="s">
         <v>49</v>
       </c>
@@ -2998,13 +3022,13 @@
       <c r="E18" s="48"/>
       <c r="F18" s="49"/>
     </row>
-    <row r="21" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="14" thickBot="1"/>
+    <row r="22" spans="2:6" ht="14" thickBot="1">
       <c r="B22" s="44" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="B23" s="50" t="s">
         <v>42</v>
       </c>
@@ -3021,7 +3045,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" ht="80" customHeight="1">
       <c r="B24" s="42" t="s">
         <v>46</v>
       </c>
@@ -3030,7 +3054,7 @@
       <c r="E24" s="36"/>
       <c r="F24" s="46"/>
     </row>
-    <row r="25" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" ht="80" customHeight="1">
       <c r="B25" s="42" t="s">
         <v>47</v>
       </c>
@@ -3039,7 +3063,7 @@
       <c r="E25" s="36"/>
       <c r="F25" s="46"/>
     </row>
-    <row r="26" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" ht="80" customHeight="1">
       <c r="B26" s="42" t="s">
         <v>48</v>
       </c>
@@ -3048,7 +3072,7 @@
       <c r="E26" s="36"/>
       <c r="F26" s="46"/>
     </row>
-    <row r="27" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B27" s="43" t="s">
         <v>49</v>
       </c>
@@ -3057,14 +3081,14 @@
       <c r="E27" s="48"/>
       <c r="F27" s="49"/>
     </row>
-    <row r="30" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="14" thickBot="1"/>
+    <row r="31" spans="2:6" ht="14" thickBot="1">
       <c r="B31" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C31" s="54"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6">
       <c r="B32" s="55" t="s">
         <v>42</v>
       </c>
@@ -3081,7 +3105,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" ht="80" customHeight="1">
       <c r="B33" s="42" t="s">
         <v>46</v>
       </c>
@@ -3090,7 +3114,7 @@
       <c r="E33" s="36"/>
       <c r="F33" s="46"/>
     </row>
-    <row r="34" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:6" ht="80" customHeight="1">
       <c r="B34" s="42" t="s">
         <v>47</v>
       </c>
@@ -3099,7 +3123,7 @@
       <c r="E34" s="36"/>
       <c r="F34" s="46"/>
     </row>
-    <row r="35" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:6" ht="80" customHeight="1">
       <c r="B35" s="42" t="s">
         <v>48</v>
       </c>
@@ -3108,7 +3132,7 @@
       <c r="E35" s="36"/>
       <c r="F35" s="46"/>
     </row>
-    <row r="36" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B36" s="43" t="s">
         <v>49</v>
       </c>
@@ -3117,14 +3141,14 @@
       <c r="E36" s="48"/>
       <c r="F36" s="49"/>
     </row>
-    <row r="39" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="2:6" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="14" thickBot="1"/>
+    <row r="40" spans="2:6" ht="14" thickBot="1">
       <c r="B40" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C40" s="54"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:6">
       <c r="B41" s="55" t="s">
         <v>42</v>
       </c>
@@ -3141,7 +3165,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:6" ht="80" customHeight="1">
       <c r="B42" s="42" t="s">
         <v>46</v>
       </c>
@@ -3150,7 +3174,7 @@
       <c r="E42" s="36"/>
       <c r="F42" s="46"/>
     </row>
-    <row r="43" spans="2:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:6" ht="80" customHeight="1">
       <c r="B43" s="42" t="s">
         <v>47</v>
       </c>
@@ -3159,7 +3183,7 @@
       <c r="E43" s="36"/>
       <c r="F43" s="46"/>
     </row>
-    <row r="44" spans="2:6" ht="67.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:6" ht="68" customHeight="1">
       <c r="B44" s="42" t="s">
         <v>48</v>
       </c>
@@ -3168,7 +3192,7 @@
       <c r="E44" s="36"/>
       <c r="F44" s="46"/>
     </row>
-    <row r="45" spans="2:6" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" ht="80" customHeight="1" thickBot="1">
       <c r="B45" s="43" t="s">
         <v>49</v>
       </c>

</xml_diff>